<commit_message>
add id logs for maianthemum curves
</commit_message>
<xml_diff>
--- a/log/2023_curve_samplesize_by_spp.xlsx
+++ b/log/2023_curve_samplesize_by_spp.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/trillium_trail/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{815B86D3-7309-6D4C-92D0-EA7511E74F39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19063AE5-7452-1048-AAF4-3C4DE3CF7F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="27640" windowHeight="15360" xr2:uid="{8D3DFF3C-B526-6E43-9345-301357687343}"/>
+    <workbookView xWindow="1600" yWindow="500" windowWidth="27640" windowHeight="15360" xr2:uid="{8D3DFF3C-B526-6E43-9345-301357687343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>spp</t>
   </si>
@@ -424,7 +426,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,6 +488,12 @@
       <c r="B3">
         <v>29</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
       <c r="G3">
         <f t="shared" ref="G3:G4" si="0">SUM(B3:F3)</f>
         <v>29</v>

</xml_diff>

<commit_message>
add second campaign logs, explore sample effort
</commit_message>
<xml_diff>
--- a/log/2023_curve_samplesize_by_spp.xlsx
+++ b/log/2023_curve_samplesize_by_spp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/trillium_trail/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19063AE5-7452-1048-AAF4-3C4DE3CF7F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03758CB-621B-D84A-B42C-DAB9F7028EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="500" windowWidth="27640" windowHeight="15360" xr2:uid="{8D3DFF3C-B526-6E43-9345-301357687343}"/>
+    <workbookView xWindow="2940" yWindow="500" windowWidth="41920" windowHeight="28300" xr2:uid="{8D3DFF3C-B526-6E43-9345-301357687343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>spp</t>
   </si>
@@ -72,13 +72,49 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Trillium grandiflorum</t>
+  </si>
+  <si>
+    <t>Maianthemum racemosum</t>
+  </si>
+  <si>
+    <t>Arisaema triphyllum</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Canopy status</t>
+  </si>
+  <si>
+    <t>Weeded</t>
+  </si>
+  <si>
+    <t>Invaded</t>
+  </si>
+  <si>
+    <t>Plot 3</t>
+  </si>
+  <si>
+    <t>Plot 5</t>
+  </si>
+  <si>
+    <t>Plot 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,16 +122,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -103,12 +165,219 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,121 +692,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B43610-06F8-4B4D-844F-303C0FA04B10}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="362" zoomScaleNormal="362" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <f>4+8+3+7</f>
         <v>22</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
         <f>17+17</f>
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
         <f>11+11</f>
         <v>22</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <f>SUM(B2:F2)</f>
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
         <f t="shared" ref="G3:G4" si="0">SUM(B3:F3)</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <f>SUM(B2:B4)</f>
         <v>51</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f t="shared" ref="C5:G5" si="1">SUM(C2:C4)</f>
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-    </row>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="6">
+        <v>10</v>
+      </c>
+      <c r="D14" s="7">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6">
+        <v>20</v>
+      </c>
+      <c r="F14" s="7">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6">
+        <v>6</v>
+      </c>
+      <c r="H14" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5">
+        <v>11</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4">
+        <v>14</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4</v>
+      </c>
+      <c r="F16" s="4">
+        <v>7</v>
+      </c>
+      <c r="G16" s="2">
+        <v>17</v>
+      </c>
+      <c r="H16" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="3">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5">
+        <v>6</v>
+      </c>
+      <c r="G17" s="3">
+        <v>9</v>
+      </c>
+      <c r="H17" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="12">
+        <v>4</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="12">
+        <v>7</v>
+      </c>
+      <c r="H19" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A14:A15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>